<commit_message>
falta por hacer cuando se elimina el segundo y el tercero estado futuro
</commit_message>
<xml_diff>
--- a/Algoritmos.xlsx
+++ b/Algoritmos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAFEYEF\OneDrive\Escritorio\Programas Pipe\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAFEYEF\OneDrive\Escritorio\Programas Pipe\TallerAlgoritmos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -337,10 +337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -388,6 +388,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>